<commit_message>
Hatali Mosfet paketi duzeltildi. EMI filtre kaldirildi ve kart boyu kisaldi. TO247-2 paketli boost diyodu kullanildi.
</commit_message>
<xml_diff>
--- a/Control/control_module_bom_.xlsx
+++ b/Control/control_module_bom_.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiCAD\Projects\PFC2k5W\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CC02F066-1191-454E-9139-3F169F9F9986}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65822482-C095-4C55-930E-94ACF0E52C90}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="control_module_bom_" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -726,10 +726,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1085,11 +1086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,10 +1276,10 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1455,7 +1456,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{F5267C55-9F49-4548-9F74-CC97A6C0B518}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{874DC08B-D0B5-4D23-85F6-76E970229D71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>